<commit_message>
need to complete and solve list as arg in Vehicle
</commit_message>
<xml_diff>
--- a/Design.xlsx
+++ b/Design.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -91,9 +91,6 @@
     <t>Red</t>
   </si>
   <si>
-    <t>Whit</t>
-  </si>
-  <si>
     <t>Black</t>
   </si>
   <si>
@@ -220,9 +217,6 @@
     <t>אופציה ב :</t>
   </si>
   <si>
-    <t>3DoorsCuppe</t>
-  </si>
-  <si>
     <t>PrintMenu : void</t>
   </si>
   <si>
@@ -257,6 +251,12 @@
   </si>
   <si>
     <t>MaxEnergy : float</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>TreeDoorCuppe</t>
   </si>
 </sst>
 </file>
@@ -448,7 +448,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -476,6 +476,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" readingOrder="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -928,23 +931,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U31" sqref="U31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="8" max="8" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.19921875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.25" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" customWidth="1"/>
-    <col min="15" max="15" width="37.19921875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="27.59765625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.296875" customWidth="1"/>
-    <col min="19" max="19" width="36.296875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="37.19921875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="37.25" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="27.625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.25" customWidth="1"/>
+    <col min="19" max="19" width="36.25" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="37.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="13"/>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -957,7 +960,7 @@
       <c r="J1" s="14"/>
       <c r="K1" s="15"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="16"/>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -965,14 +968,14 @@
       <c r="E2" s="17"/>
       <c r="F2" s="17"/>
       <c r="G2" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H2" s="17"/>
       <c r="I2" s="17"/>
       <c r="J2" s="17"/>
       <c r="K2" s="18"/>
     </row>
-    <row r="3" spans="1:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
@@ -985,7 +988,7 @@
       <c r="J3" s="17"/>
       <c r="K3" s="18"/>
     </row>
-    <row r="4" spans="1:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
       <c r="B4" s="17"/>
       <c r="C4" s="17"/>
@@ -999,18 +1002,24 @@
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
+      <c r="L4">
+        <v>1</v>
+      </c>
       <c r="M4" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
       <c r="O4" s="5" t="s">
         <v>12</v>
       </c>
       <c r="R4" s="3"/>
       <c r="S4" s="23" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="16"/>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
@@ -1030,10 +1039,10 @@
       </c>
       <c r="R5" s="3"/>
       <c r="S5" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
@@ -1052,10 +1061,10 @@
         <v>5</v>
       </c>
       <c r="S6" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
@@ -1073,14 +1082,17 @@
       <c r="O7" s="7" t="s">
         <v>6</v>
       </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
       <c r="Q7" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S7" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -1099,13 +1111,13 @@
         <v>11</v>
       </c>
       <c r="Q8" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="S8" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -1124,16 +1136,16 @@
       <c r="J9" s="17"/>
       <c r="K9" s="18"/>
       <c r="O9" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q9" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="S9" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
@@ -1145,17 +1157,20 @@
       <c r="I10" s="17"/>
       <c r="J10" s="17"/>
       <c r="K10" s="18"/>
+      <c r="L10">
+        <v>1</v>
+      </c>
       <c r="M10" s="4" t="s">
         <v>14</v>
       </c>
       <c r="O10" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q10" s="22" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
@@ -1171,11 +1186,11 @@
         <v>24</v>
       </c>
       <c r="O11" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q11" s="17"/>
     </row>
-    <row r="12" spans="1:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="24"/>
       <c r="B12" s="25"/>
       <c r="C12" s="25"/>
@@ -1188,227 +1203,242 @@
       <c r="J12" s="25"/>
       <c r="K12" s="26"/>
       <c r="M12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q12" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="S12" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Q12" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="S12" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M13" s="1" t="s">
+      <c r="Q13" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="S13" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Q13" s="20" t="s">
+      <c r="Q14" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="S13" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q14" s="21" t="s">
-        <v>50</v>
-      </c>
       <c r="S14" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="Q15" s="22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="S15" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <v>1</v>
+      </c>
       <c r="M16" s="4" t="s">
         <v>20</v>
       </c>
       <c r="Q16" s="17"/>
       <c r="S16" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="13:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="Q17" s="19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="S17" s="10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="13:19" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="12:19" x14ac:dyDescent="0.2">
       <c r="M18" s="1" t="s">
         <v>21</v>
       </c>
       <c r="Q18" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S18" s="10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="13:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M19" s="2" t="s">
         <v>22</v>
       </c>
       <c r="Q19" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="S19" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q20" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="S20" s="11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="13:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q20" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="S20" s="11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="13:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="N21">
+        <v>1</v>
+      </c>
       <c r="O21" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="13:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L22">
+        <v>1</v>
+      </c>
       <c r="M22" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O22" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="13:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M23" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O23" s="7" t="s">
         <v>8</v>
       </c>
       <c r="S23" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="13:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M24" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O24" s="7" t="s">
         <v>9</v>
       </c>
       <c r="S24" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="13:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M25" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O25" s="8" t="s">
         <v>10</v>
       </c>
       <c r="S25" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="26" spans="13:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q26" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="S26" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M27" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="Q26" s="5" t="s">
+      <c r="Q27" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="S26" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="27" spans="13:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M27" s="1" t="s">
+      <c r="S27" s="10"/>
+    </row>
+    <row r="28" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M28" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="Q27" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="S27" s="10"/>
-    </row>
-    <row r="28" spans="13:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M28" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="Q28" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="S28" s="10"/>
     </row>
-    <row r="29" spans="13:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="S29" s="10"/>
     </row>
-    <row r="30" spans="13:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L30">
+        <v>1</v>
+      </c>
       <c r="M30" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S30" s="10"/>
     </row>
-    <row r="31" spans="13:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M31" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S31" s="11"/>
+    </row>
+    <row r="32" spans="12:19" x14ac:dyDescent="0.2">
+      <c r="M32" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="S31" s="11"/>
-    </row>
-    <row r="32" spans="13:19" x14ac:dyDescent="0.25">
-      <c r="M32" s="1" t="s">
+    </row>
+    <row r="33" spans="12:15" x14ac:dyDescent="0.2">
+      <c r="M33" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="13:15" x14ac:dyDescent="0.25">
-      <c r="M33" s="1" t="s">
+    <row r="34" spans="12:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M34" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="13:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M34" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="35" spans="13:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="12:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="O35" s="3"/>
     </row>
-    <row r="36" spans="13:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="12:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L36">
+        <v>1</v>
+      </c>
       <c r="M36" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="O36" s="3"/>
+    </row>
+    <row r="37" spans="12:15" x14ac:dyDescent="0.2">
+      <c r="M37" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="O36" s="3"/>
-    </row>
-    <row r="37" spans="13:15" x14ac:dyDescent="0.25">
-      <c r="M37" s="1" t="s">
+    </row>
+    <row r="38" spans="12:15" x14ac:dyDescent="0.2">
+      <c r="M38" s="27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="12:15" x14ac:dyDescent="0.2">
+      <c r="M39" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="13:15" x14ac:dyDescent="0.25">
-      <c r="M38" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="39" spans="13:15" x14ac:dyDescent="0.25">
-      <c r="M39" s="1" t="s">
+    <row r="40" spans="12:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M40" s="2" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="40" spans="13:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M40" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish skeleton, finish implement Garage, need to fix Vehicle cntr
</commit_message>
<xml_diff>
--- a/Design.xlsx
+++ b/Design.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="80">
   <si>
     <t>VEHICLE</t>
   </si>
@@ -196,9 +196,6 @@
     <t>ChangeVehicleState(LPN, NewState)</t>
   </si>
   <si>
-    <t>ShowAllLPNByState (State)</t>
-  </si>
-  <si>
     <t>ChargeElectricCar(LPN, MinutesToCharge)</t>
   </si>
   <si>
@@ -211,9 +208,6 @@
     <t>FillAllWheelsToMaxPressure()</t>
   </si>
   <si>
-    <t>ShowVehicleDetails(LPN)</t>
-  </si>
-  <si>
     <t>אופציה ב :</t>
   </si>
   <si>
@@ -229,9 +223,6 @@
     <t>Energy : Energy</t>
   </si>
   <si>
-    <t>Energy : Energy(Fueled)</t>
-  </si>
-  <si>
     <t>VehicleGenerator</t>
   </si>
   <si>
@@ -241,9 +232,6 @@
     <t>AddVehicle</t>
   </si>
   <si>
-    <t>getVehicle</t>
-  </si>
-  <si>
     <t>Truck : Class</t>
   </si>
   <si>
@@ -257,6 +245,15 @@
   </si>
   <si>
     <t>TreeDoorCuppe</t>
+  </si>
+  <si>
+    <t>GetVehicleByLPN</t>
+  </si>
+  <si>
+    <t>GetVehicleForDetails(LPN)</t>
+  </si>
+  <si>
+    <t>GetAllVehicleLPNByState (State)</t>
   </si>
 </sst>
 </file>
@@ -931,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -968,7 +965,7 @@
       <c r="E2" s="17"/>
       <c r="F2" s="17"/>
       <c r="G2" s="17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H2" s="17"/>
       <c r="I2" s="17"/>
@@ -1011,12 +1008,14 @@
       <c r="N4">
         <v>1</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="O4" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="R4" s="3"/>
+      <c r="R4" s="3">
+        <v>1</v>
+      </c>
       <c r="S4" s="23" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -1039,7 +1038,7 @@
       </c>
       <c r="R5" s="3"/>
       <c r="S5" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1089,7 +1088,7 @@
         <v>44</v>
       </c>
       <c r="S7" s="7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1114,7 +1113,7 @@
         <v>45</v>
       </c>
       <c r="S8" s="8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1138,7 +1137,7 @@
       <c r="O9" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="Q9" s="21" t="s">
+      <c r="Q9" s="22" t="s">
         <v>52</v>
       </c>
       <c r="S9" s="11" t="s">
@@ -1163,11 +1162,8 @@
       <c r="M10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="O10" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q10" s="22" t="s">
-        <v>70</v>
+      <c r="O10" s="21" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1185,8 +1181,8 @@
       <c r="M11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="O11" s="12" t="s">
-        <v>42</v>
+      <c r="O11" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="Q11" s="17"/>
     </row>
@@ -1203,7 +1199,13 @@
       <c r="J12" s="25"/>
       <c r="K12" s="26"/>
       <c r="M12" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
+      </c>
+      <c r="O12" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
       </c>
       <c r="Q12" s="19" t="s">
         <v>46</v>
@@ -1220,14 +1222,14 @@
         <v>48</v>
       </c>
       <c r="S13" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Q14" s="21" t="s">
+      <c r="Q14" s="22" t="s">
         <v>49</v>
       </c>
       <c r="S14" s="9" t="s">
@@ -1235,11 +1237,12 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="Q15" s="22" t="s">
-        <v>70</v>
+      <c r="Q15" s="17"/>
+      <c r="R15">
+        <v>1</v>
       </c>
       <c r="S15" s="10" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1249,50 +1252,64 @@
       <c r="M16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="Q16" s="17"/>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="R16">
+        <v>1</v>
+      </c>
       <c r="S16" s="10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="12:19" x14ac:dyDescent="0.2">
       <c r="M17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Q17" s="19" t="s">
-        <v>76</v>
+      <c r="Q17" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="R17">
+        <v>1</v>
       </c>
       <c r="S17" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="12:19" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Q18" s="20" t="s">
-        <v>50</v>
+      <c r="Q18" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="R18">
+        <v>1</v>
       </c>
       <c r="S18" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M19" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Q19" s="21" t="s">
-        <v>51</v>
+      <c r="R19">
+        <v>1</v>
       </c>
       <c r="S19" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="Q20" s="22" t="s">
-        <v>71</v>
+      <c r="R20">
+        <v>1</v>
       </c>
       <c r="S20" s="11" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1322,7 +1339,7 @@
         <v>8</v>
       </c>
       <c r="S23" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1332,8 +1349,14 @@
       <c r="O24" s="7" t="s">
         <v>9</v>
       </c>
+      <c r="Q24" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="R24">
+        <v>1</v>
+      </c>
       <c r="S24" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1343,27 +1366,30 @@
       <c r="O25" s="8" t="s">
         <v>10</v>
       </c>
+      <c r="Q25" s="7" t="s">
+        <v>57</v>
+      </c>
       <c r="S25" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Q26" s="5" t="s">
-        <v>56</v>
+      <c r="Q26" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="R26">
+        <v>1</v>
       </c>
       <c r="S26" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="27" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="12:19" x14ac:dyDescent="0.2">
       <c r="M27" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="Q27" s="7" t="s">
-        <v>57</v>
       </c>
       <c r="S27" s="10"/>
     </row>
@@ -1371,9 +1397,6 @@
       <c r="M28" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="Q28" s="12" t="s">
-        <v>67</v>
-      </c>
       <c r="S28" s="10"/>
     </row>
     <row r="29" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1428,7 +1451,7 @@
     </row>
     <row r="38" spans="12:15" x14ac:dyDescent="0.2">
       <c r="M38" s="27" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="12:15" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added logic to create vehicls
</commit_message>
<xml_diff>
--- a/Design.xlsx
+++ b/Design.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
   <si>
     <t>VEHICLE</t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>LPN :string</t>
-  </si>
-  <si>
-    <t>AmountOfEnergy : float</t>
   </si>
   <si>
     <t>ManufactureName : string</t>
@@ -928,8 +925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -965,7 +962,7 @@
       <c r="E2" s="17"/>
       <c r="F2" s="17"/>
       <c r="G2" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H2" s="17"/>
       <c r="I2" s="17"/>
@@ -1003,19 +1000,19 @@
         <v>1</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N4">
         <v>1</v>
       </c>
       <c r="O4" s="23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R4" s="3">
         <v>1</v>
       </c>
       <c r="S4" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -1031,14 +1028,14 @@
       <c r="J5" s="17"/>
       <c r="K5" s="18"/>
       <c r="M5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O5" s="6" t="s">
         <v>4</v>
       </c>
       <c r="R5" s="3"/>
       <c r="S5" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1054,13 +1051,13 @@
       <c r="J6" s="17"/>
       <c r="K6" s="18"/>
       <c r="M6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O6" s="7" t="s">
         <v>5</v>
       </c>
       <c r="S6" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1076,19 +1073,17 @@
       <c r="J7" s="17"/>
       <c r="K7" s="18"/>
       <c r="M7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O7" s="7" t="s">
-        <v>6</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="O7" s="7"/>
       <c r="P7">
         <v>0</v>
       </c>
       <c r="Q7" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="S7" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1104,16 +1099,16 @@
       <c r="J8" s="17"/>
       <c r="K8" s="18"/>
       <c r="M8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O8" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q8" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S8" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1135,13 +1130,13 @@
       <c r="J9" s="17"/>
       <c r="K9" s="18"/>
       <c r="O9" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q9" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="S9" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1160,10 +1155,10 @@
         <v>1</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O10" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1179,10 +1174,10 @@
       <c r="J11" s="17"/>
       <c r="K11" s="18"/>
       <c r="M11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O11" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q11" s="17"/>
     </row>
@@ -1199,41 +1194,41 @@
       <c r="J12" s="25"/>
       <c r="K12" s="26"/>
       <c r="M12" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O12" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P12">
         <v>0</v>
       </c>
       <c r="Q12" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="S12" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q13" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S13" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M14" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q14" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="S14" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1242,7 +1237,7 @@
         <v>1</v>
       </c>
       <c r="S15" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1250,58 +1245,58 @@
         <v>1</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P16">
         <v>0</v>
       </c>
       <c r="Q16" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R16">
         <v>1</v>
       </c>
       <c r="S16" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="12:19" x14ac:dyDescent="0.2">
       <c r="M17" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q17" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="R17">
         <v>1</v>
       </c>
       <c r="S17" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M18" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q18" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="R18">
         <v>1</v>
       </c>
       <c r="S18" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M19" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R19">
         <v>1</v>
       </c>
       <c r="S19" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1309,7 +1304,7 @@
         <v>1</v>
       </c>
       <c r="S20" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1317,7 +1312,7 @@
         <v>1</v>
       </c>
       <c r="O21" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1325,77 +1320,77 @@
         <v>1</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O22" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M23" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O23" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="S23" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M24" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O24" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q24" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R24">
         <v>1</v>
       </c>
       <c r="S24" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M25" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O25" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q25" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="S25" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M26" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q26" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="R26">
         <v>1</v>
       </c>
       <c r="S26" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="12:19" x14ac:dyDescent="0.2">
       <c r="M27" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S27" s="10"/>
     </row>
     <row r="28" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M28" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S28" s="10"/>
     </row>
@@ -1407,29 +1402,29 @@
         <v>1</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S30" s="10"/>
     </row>
     <row r="31" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M31" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S31" s="11"/>
     </row>
     <row r="32" spans="12:19" x14ac:dyDescent="0.2">
       <c r="M32" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="12:15" x14ac:dyDescent="0.2">
       <c r="M33" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="12:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M34" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="12:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1440,28 +1435,28 @@
         <v>1</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O36" s="3"/>
     </row>
     <row r="37" spans="12:15" x14ac:dyDescent="0.2">
       <c r="M37" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="12:15" x14ac:dyDescent="0.2">
       <c r="M38" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="12:15" x14ac:dyDescent="0.2">
       <c r="M39" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="12:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M40" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added powerpoint and word doc.
</commit_message>
<xml_diff>
--- a/Design.xlsx
+++ b/Design.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="92">
   <si>
     <t>VEHICLE</t>
   </si>
@@ -251,6 +251,45 @@
   </si>
   <si>
     <t>GetAllVehicleLPNByState (State)</t>
+  </si>
+  <si>
+    <t>+ ToString()</t>
+  </si>
+  <si>
+    <t>+ Vehicle()</t>
+  </si>
+  <si>
+    <t>+ FillEnergy()</t>
+  </si>
+  <si>
+    <t>+ FillAirToMaxPressure()</t>
+  </si>
+  <si>
+    <t>+ GetGeneralDetails()</t>
+  </si>
+  <si>
+    <t>- m_LPN</t>
+  </si>
+  <si>
+    <t>- m_Model</t>
+  </si>
+  <si>
+    <t>- m_Wheels</t>
+  </si>
+  <si>
+    <t>- m_OwnerName</t>
+  </si>
+  <si>
+    <t>- m_OwnerPhoneNumber</t>
+  </si>
+  <si>
+    <t>- m_Energy</t>
+  </si>
+  <si>
+    <t>Vehicle</t>
+  </si>
+  <si>
+    <t>- m_VehicleState</t>
   </si>
 </sst>
 </file>
@@ -442,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -473,6 +512,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" readingOrder="2"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -631,6 +674,44 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>4843</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>93228</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2749826" y="3023152"/>
+          <a:ext cx="2067213" cy="3315163"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -925,13 +1006,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="8" max="8" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.25" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" customWidth="1"/>
     <col min="15" max="15" width="37.25" bestFit="1" customWidth="1"/>
@@ -1260,7 +1342,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="12:19" x14ac:dyDescent="0.2">
+    <row r="17" spans="9:19" x14ac:dyDescent="0.2">
       <c r="M17" s="1" t="s">
         <v>22</v>
       </c>
@@ -1274,7 +1356,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M18" s="1" t="s">
         <v>20</v>
       </c>
@@ -1288,7 +1370,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M19" s="2" t="s">
         <v>21</v>
       </c>
@@ -1299,7 +1381,10 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I20" s="31" t="s">
+        <v>90</v>
+      </c>
       <c r="R20">
         <v>1</v>
       </c>
@@ -1307,7 +1392,10 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I21" s="28" t="s">
+        <v>85</v>
+      </c>
       <c r="N21">
         <v>1</v>
       </c>
@@ -1315,7 +1403,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I22" s="29" t="s">
+        <v>84</v>
+      </c>
       <c r="L22">
         <v>1</v>
       </c>
@@ -1326,7 +1417,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I23" s="29" t="s">
+        <v>86</v>
+      </c>
       <c r="M23" s="1" t="s">
         <v>28</v>
       </c>
@@ -1337,7 +1431,10 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I24" s="29" t="s">
+        <v>87</v>
+      </c>
       <c r="M24" s="1" t="s">
         <v>27</v>
       </c>
@@ -1354,7 +1451,10 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I25" s="29" t="s">
+        <v>88</v>
+      </c>
       <c r="M25" s="1" t="s">
         <v>29</v>
       </c>
@@ -1368,7 +1468,10 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I26" s="29" t="s">
+        <v>89</v>
+      </c>
       <c r="M26" s="1" t="s">
         <v>30</v>
       </c>
@@ -1382,22 +1485,34 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="12:19" x14ac:dyDescent="0.2">
+    <row r="27" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I27" s="30" t="s">
+        <v>91</v>
+      </c>
       <c r="M27" s="1" t="s">
         <v>31</v>
       </c>
       <c r="S27" s="10"/>
     </row>
-    <row r="28" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I28" s="28" t="s">
+        <v>79</v>
+      </c>
       <c r="M28" s="2" t="s">
         <v>32</v>
       </c>
       <c r="S28" s="10"/>
     </row>
-    <row r="29" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I29" s="29" t="s">
+        <v>80</v>
+      </c>
       <c r="S29" s="10"/>
     </row>
-    <row r="30" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I30" s="29" t="s">
+        <v>81</v>
+      </c>
       <c r="L30">
         <v>1</v>
       </c>
@@ -1406,13 +1521,19 @@
       </c>
       <c r="S30" s="10"/>
     </row>
-    <row r="31" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I31" s="29" t="s">
+        <v>82</v>
+      </c>
       <c r="M31" s="1" t="s">
         <v>36</v>
       </c>
       <c r="S31" s="11"/>
     </row>
-    <row r="32" spans="12:19" x14ac:dyDescent="0.2">
+    <row r="32" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I32" s="30" t="s">
+        <v>83</v>
+      </c>
       <c r="M32" s="1" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
finished word + powerpoint files - ready to sent
</commit_message>
<xml_diff>
--- a/Design.xlsx
+++ b/Design.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="104">
   <si>
     <t>VEHICLE</t>
   </si>
@@ -290,14 +290,58 @@
   </si>
   <si>
     <t>- m_VehicleState</t>
+  </si>
+  <si>
+    <t>Car</t>
+  </si>
+  <si>
+    <t>- m_Color</t>
+  </si>
+  <si>
+    <t>- m_NumberOfDoors</t>
+  </si>
+  <si>
+    <t>- k_ManufactureMaxPressure</t>
+  </si>
+  <si>
+    <t>+ car()</t>
+  </si>
+  <si>
+    <t>Truck</t>
+  </si>
+  <si>
+    <t>- m_CargoVolume</t>
+  </si>
+  <si>
+    <t>- m_IsDangerousMaterials</t>
+  </si>
+  <si>
+    <t>+ Truck()</t>
+  </si>
+  <si>
+    <t>MotorCycle</t>
+  </si>
+  <si>
+    <t>- m_License</t>
+  </si>
+  <si>
+    <t>- m_EngineVolume</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -481,7 +525,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -515,7 +559,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -678,16 +728,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>240195</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>115956</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>4843</xdr:colOff>
+      <xdr:colOff>1619951</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>93228</xdr:rowOff>
+      <xdr:rowOff>184336</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -704,8 +754,46 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2749826" y="3023152"/>
+          <a:off x="4364934" y="3139108"/>
           <a:ext cx="2067213" cy="3315163"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1570283</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>68141</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3205370"/>
+          <a:ext cx="2257740" cy="1600423"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1006,12 +1094,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.25" bestFit="1" customWidth="1"/>
@@ -1342,7 +1432,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="9:19" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:19" x14ac:dyDescent="0.2">
       <c r="M17" s="1" t="s">
         <v>22</v>
       </c>
@@ -1356,7 +1446,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M18" s="1" t="s">
         <v>20</v>
       </c>
@@ -1370,7 +1460,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M19" s="2" t="s">
         <v>21</v>
       </c>
@@ -1381,7 +1471,10 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E20" s="33" t="s">
+        <v>92</v>
+      </c>
       <c r="I20" s="31" t="s">
         <v>90</v>
       </c>
@@ -1392,7 +1485,10 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E21" s="28" t="s">
+        <v>93</v>
+      </c>
       <c r="I21" s="28" t="s">
         <v>85</v>
       </c>
@@ -1403,7 +1499,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E22" s="29" t="s">
+        <v>94</v>
+      </c>
       <c r="I22" s="29" t="s">
         <v>84</v>
       </c>
@@ -1417,7 +1516,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E23" s="30" t="s">
+        <v>95</v>
+      </c>
       <c r="I23" s="29" t="s">
         <v>86</v>
       </c>
@@ -1431,7 +1533,10 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E24" s="29" t="s">
+        <v>79</v>
+      </c>
       <c r="I24" s="29" t="s">
         <v>87</v>
       </c>
@@ -1451,7 +1556,10 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E25" s="30" t="s">
+        <v>96</v>
+      </c>
       <c r="I25" s="29" t="s">
         <v>88</v>
       </c>
@@ -1468,7 +1576,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E26" s="32"/>
       <c r="I26" s="29" t="s">
         <v>89</v>
       </c>
@@ -1485,7 +1594,8 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E27" s="32"/>
       <c r="I27" s="30" t="s">
         <v>91</v>
       </c>
@@ -1494,7 +1604,8 @@
       </c>
       <c r="S27" s="10"/>
     </row>
-    <row r="28" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E28" s="32"/>
       <c r="I28" s="28" t="s">
         <v>79</v>
       </c>
@@ -1503,13 +1614,20 @@
       </c>
       <c r="S28" s="10"/>
     </row>
-    <row r="29" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E29" s="32"/>
       <c r="I29" s="29" t="s">
         <v>80</v>
       </c>
       <c r="S29" s="10"/>
     </row>
-    <row r="30" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="E30" s="33" t="s">
+        <v>97</v>
+      </c>
       <c r="I30" s="29" t="s">
         <v>81</v>
       </c>
@@ -1521,7 +1639,13 @@
       </c>
       <c r="S30" s="10"/>
     </row>
-    <row r="31" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="E31" s="28" t="s">
+        <v>98</v>
+      </c>
       <c r="I31" s="29" t="s">
         <v>82</v>
       </c>
@@ -1530,7 +1654,13 @@
       </c>
       <c r="S31" s="11"/>
     </row>
-    <row r="32" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="E32" s="29" t="s">
+        <v>99</v>
+      </c>
       <c r="I32" s="30" t="s">
         <v>83</v>
       </c>
@@ -1538,20 +1668,38 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="12:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="E33" s="30" t="s">
+        <v>95</v>
+      </c>
       <c r="M33" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="12:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="E34" s="29" t="s">
+        <v>79</v>
+      </c>
       <c r="M34" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="12:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="E35" s="30" t="s">
+        <v>100</v>
+      </c>
       <c r="O35" s="3"/>
     </row>
-    <row r="36" spans="12:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="L36">
         <v>1</v>
       </c>
@@ -1560,22 +1708,22 @@
       </c>
       <c r="O36" s="3"/>
     </row>
-    <row r="37" spans="12:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:15" x14ac:dyDescent="0.2">
       <c r="M37" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="12:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:15" x14ac:dyDescent="0.2">
       <c r="M38" s="27" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="12:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:15" x14ac:dyDescent="0.2">
       <c r="M39" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="12:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M40" s="2" t="s">
         <v>54</v>
       </c>

</xml_diff>